<commit_message>
final Filter und display
</commit_message>
<xml_diff>
--- a/pythonProject2/Schiffsreisen_cleaned.xlsx
+++ b/pythonProject2/Schiffsreisen_cleaned.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GUI\test\pythonProject2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GUI\GUI_projekt\pythonProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ED80FD-F7EE-4AA7-8FC8-1F334FB79C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BA58F-2B47-4132-BD4A-BBDB8DD17B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1194,28 +1194,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="94.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="94.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>4250</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1740,209 +1740,240 @@
         <v>4999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" t="s">
+        <v>175</v>
+      </c>
+      <c r="H16" t="s">
+        <v>216</v>
+      </c>
+      <c r="I16" t="s">
+        <v>247</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2015</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J17" s="2">
-        <v>2015</v>
+        <v>3025</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
         <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J18" s="2">
-        <v>3025</v>
+        <v>3249</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I19" t="s">
-        <v>249</v>
-      </c>
-      <c r="J19" s="2">
-        <v>3249</v>
+        <v>132</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
         <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I21" t="s">
-        <v>250</v>
+        <v>132</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K21" s="2">
-        <v>3478</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="G22" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I22" t="s">
         <v>132</v>
@@ -1954,53 +1985,53 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G23" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="H23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I23" t="s">
-        <v>132</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5910</v>
+      </c>
+      <c r="K23" s="2">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E24" t="s">
         <v>117</v>
@@ -2009,753 +2040,815 @@
         <v>132</v>
       </c>
       <c r="G24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H24" t="s">
-        <v>223</v>
+        <v>162</v>
       </c>
       <c r="I24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J24" s="2">
-        <v>5910</v>
+        <v>3950</v>
       </c>
       <c r="K24" s="2">
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="G25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="I25" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J25" s="2">
-        <v>3950</v>
+        <v>4390</v>
       </c>
       <c r="K25" s="2">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G26" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="H26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I26" t="s">
-        <v>253</v>
+        <v>195</v>
       </c>
       <c r="J26" s="2">
-        <v>4390</v>
+        <v>4000</v>
       </c>
       <c r="K26" s="2">
-        <v>4999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G27" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="H27" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I27" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="J27" s="2">
-        <v>4000</v>
+        <v>3850</v>
       </c>
       <c r="K27" s="2">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H28" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="I28" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J28" s="2">
-        <v>3850</v>
+        <v>3890</v>
       </c>
       <c r="K28" s="2">
-        <v>3990</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
       <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G29" t="s">
+        <v>186</v>
+      </c>
+      <c r="H29" t="s">
+        <v>158</v>
+      </c>
+      <c r="I29" t="s">
+        <v>231</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2800</v>
+      </c>
+      <c r="K29" s="2">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" t="s">
-        <v>144</v>
-      </c>
-      <c r="G29" t="s">
-        <v>185</v>
-      </c>
-      <c r="H29" t="s">
-        <v>211</v>
-      </c>
-      <c r="I29" t="s">
-        <v>255</v>
-      </c>
-      <c r="J29" s="2">
-        <v>3890</v>
-      </c>
-      <c r="K29" s="2">
-        <v>3950</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>18</v>
-      </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G30" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H30" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="I30" t="s">
-        <v>231</v>
-      </c>
-      <c r="J30" s="2">
-        <v>2800</v>
+        <v>256</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="K30" s="2">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" t="s">
+        <v>188</v>
+      </c>
+      <c r="H31" t="s">
+        <v>228</v>
+      </c>
+      <c r="I31" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H32" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I32" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K32" s="2">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
         <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F33" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H33" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I33" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K33" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="2">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G34" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H34" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
+      </c>
+      <c r="J34" s="2">
+        <v>3249</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F35" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="G35" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H35" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I35" t="s">
-        <v>257</v>
+        <v>132</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K35" s="2">
-        <v>3240</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
         <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F36" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G36" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
       <c r="H36" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="I36" t="s">
-        <v>144</v>
-      </c>
-      <c r="J36" s="2">
-        <v>3249</v>
+        <v>132</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="G37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H37" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="J37" s="2">
+        <v>3900</v>
+      </c>
+      <c r="K37" s="2">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F38" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G38" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="H38" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="I38" t="s">
-        <v>132</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="J38" s="2">
+        <v>4500</v>
+      </c>
+      <c r="K38" s="2">
+        <v>5090</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H39" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I39" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J39" s="2">
-        <v>3900</v>
+        <v>4790</v>
       </c>
       <c r="K39" s="2">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F40" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="H40" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="I40" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="J40" s="2">
-        <v>4500</v>
+        <v>3580</v>
       </c>
       <c r="K40" s="2">
-        <v>5090</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F41" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G41" t="s">
+        <v>196</v>
+      </c>
+      <c r="H41" t="s">
+        <v>236</v>
+      </c>
+      <c r="I41" t="s">
         <v>195</v>
       </c>
-      <c r="H41" t="s">
-        <v>235</v>
-      </c>
-      <c r="I41" t="s">
-        <v>259</v>
-      </c>
       <c r="J41" s="2">
-        <v>4790</v>
+        <v>4050</v>
       </c>
       <c r="K41" s="2">
-        <v>5019</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
         <v>118</v>
       </c>
       <c r="F42" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G42" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="H42" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I42" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="J42" s="2">
-        <v>3580</v>
+        <v>2600</v>
       </c>
       <c r="K42" s="2">
-        <v>3790</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
         <v>119</v>
       </c>
       <c r="F43" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H43" t="s">
-        <v>236</v>
+        <v>141</v>
       </c>
       <c r="I43" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
       <c r="J43" s="2">
-        <v>4050</v>
+        <v>2790</v>
       </c>
       <c r="K43" s="2">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G44" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H44" t="s">
-        <v>145</v>
+        <v>237</v>
       </c>
       <c r="I44" t="s">
-        <v>131</v>
-      </c>
-      <c r="J44" s="2">
-        <v>2600</v>
-      </c>
-      <c r="K44" s="2">
-        <v>2699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E45" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F45" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H45" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="I45" t="s">
-        <v>260</v>
-      </c>
-      <c r="J45" s="2">
-        <v>2790</v>
-      </c>
-      <c r="K45" s="2">
-        <v>2998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G46" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" t="s">
+        <v>238</v>
+      </c>
+      <c r="I46" t="s">
+        <v>132</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
         <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F47" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G47" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H47" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="I47" t="s">
         <v>132</v>
@@ -2764,33 +2857,33 @@
         <v>132</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
         <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
         <v>122</v>
       </c>
       <c r="F48" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G48" t="s">
-        <v>200</v>
+        <v>131</v>
       </c>
       <c r="H48" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="I48" t="s">
         <v>132</v>
@@ -2799,33 +2892,33 @@
         <v>132</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
         <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G49" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="H49" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="I49" t="s">
         <v>132</v>
@@ -2834,33 +2927,33 @@
         <v>132</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E50" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="F50" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="G50" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="H50" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="I50" t="s">
         <v>132</v>
@@ -2868,34 +2961,34 @@
       <c r="J50" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K50" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="2">
+        <v>10790</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
         <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F51" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="G51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H51" t="s">
-        <v>239</v>
+        <v>132</v>
       </c>
       <c r="I51" t="s">
         <v>132</v>
@@ -2903,116 +2996,7 @@
       <c r="J51" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K51" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" t="s">
-        <v>162</v>
-      </c>
-      <c r="G52" t="s">
-        <v>202</v>
-      </c>
-      <c r="H52" t="s">
-        <v>195</v>
-      </c>
-      <c r="I52" t="s">
-        <v>132</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" t="s">
-        <v>110</v>
-      </c>
-      <c r="E54" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" t="s">
-        <v>132</v>
-      </c>
-      <c r="G54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H54" t="s">
-        <v>132</v>
-      </c>
-      <c r="I54" t="s">
-        <v>132</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K54" s="2">
-        <v>10790</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" t="s">
-        <v>111</v>
-      </c>
-      <c r="E55" t="s">
-        <v>123</v>
-      </c>
-      <c r="F55" t="s">
-        <v>132</v>
-      </c>
-      <c r="G55" t="s">
-        <v>132</v>
-      </c>
-      <c r="H55" t="s">
-        <v>132</v>
-      </c>
-      <c r="I55" t="s">
-        <v>132</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K55" s="2">
+      <c r="K51" s="2">
         <v>22500</v>
       </c>
     </row>

</xml_diff>